<commit_message>
Cleaned up exec list
</commit_message>
<xml_diff>
--- a/2009-2010/Execs.xlsx
+++ b/2009-2010/Execs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>604-761-7173</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">bluebell985622@hotmail.com </t>
-  </si>
-  <si>
-    <t>g</t>
   </si>
 </sst>
 </file>
@@ -491,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,7 +502,7 @@
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -518,11 +515,8 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -536,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -549,11 +543,8 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -567,7 +558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -580,11 +571,8 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -597,11 +585,8 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -615,7 +600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -628,11 +613,8 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -646,7 +628,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -659,11 +641,8 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -676,11 +655,8 @@
       <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -694,7 +670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -706,9 +682,6 @@
       </c>
       <c r="D13" t="s">
         <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>